<commit_message>
finished excel uploading for seasons
</commit_message>
<xml_diff>
--- a/Documents/TestExcel.xlsx
+++ b/Documents/TestExcel.xlsx
@@ -20,9 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">15/03/2019 12-12-12</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+  <si>
+    <t xml:space="preserve">15/03/2019 5:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamilton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">856 main street</t>
   </si>
   <si>
     <t xml:space="preserve">Brock 1</t>
@@ -31,35 +37,36 @@
     <t xml:space="preserve">White Oaks 1</t>
   </si>
   <si>
-    <t xml:space="preserve">09/04/2019 12-12-12</t>
+    <t xml:space="preserve">22/03/2019 12:52:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 ontario street</t>
   </si>
   <si>
     <t xml:space="preserve">Ridley 1</t>
   </si>
   <si>
-    <t xml:space="preserve">23/04/2019 12-12-12</t>
+    <t xml:space="preserve">23/04/2019 12:42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2345 king street</t>
   </si>
   <si>
     <t xml:space="preserve">BAC 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/05/2019 12-12-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28/05/2019 12-12-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16/06/2019 12-12-12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="YYYY/MM/DD\ HH:MM"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -85,57 +92,83 @@
       <charset val="128"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b val="true"/>
+      <sz val="24"/>
       <color rgb="FF000000"/>
-      <name val="Mangal"/>
-      <family val="2"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Mangal"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
-      <name val="Mangal"/>
-      <family val="2"/>
-      <charset val="128"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF808080"/>
-      <name val="Mangal"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
-      <name val="Mangal"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
-      <name val="Mangal"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
-      <name val="Mangal"/>
-      <family val="2"/>
-      <charset val="128"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Mangal"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="128"/>
     </font>
@@ -238,25 +271,61 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -353,10 +422,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E6"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="A4:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -368,66 +437,51 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>1</v>
-      </c>
       <c r="E2" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="0" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel controller uses parsexact instead of convert todatetime now
</commit_message>
<xml_diff>
--- a/Documents/TestExcel.xlsx
+++ b/Documents/TestExcel.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
-    <t xml:space="preserve">15/03/2019 5:55:00 PM</t>
+    <t xml:space="preserve">15/03/2019 5:55 PM</t>
   </si>
   <si>
     <t xml:space="preserve">Hamilton</t>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">White Oaks 1</t>
   </si>
   <si>
-    <t xml:space="preserve">22/03/2019 12:52:00 PM</t>
+    <t xml:space="preserve">22/03/2019 12:52 PM</t>
   </si>
   <si>
     <t xml:space="preserve">25 ontario street</t>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Ridley 1</t>
   </si>
   <si>
-    <t xml:space="preserve">23/04/2019 12:42:00 PM</t>
+    <t xml:space="preserve">23/04/2019 12:42 PM</t>
   </si>
   <si>
     <t xml:space="preserve">Welland</t>
@@ -427,7 +427,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Finish Excel Confirm for Seasons
</commit_message>
<xml_diff>
--- a/Documents/TestExcel.xlsx
+++ b/Documents/TestExcel.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
-    <t xml:space="preserve">15/03/2019 5:55 PM</t>
+    <t xml:space="preserve">15/03/2019</t>
   </si>
   <si>
     <t xml:space="preserve">Hamilton</t>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">White Oaks 1</t>
   </si>
   <si>
-    <t xml:space="preserve">22/03/2019 12:52 PM</t>
+    <t xml:space="preserve">22/03/2019</t>
   </si>
   <si>
     <t xml:space="preserve">25 ontario street</t>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Ridley 1</t>
   </si>
   <si>
-    <t xml:space="preserve">23/04/2019 12:42 PM</t>
+    <t xml:space="preserve">23/04/2019</t>
   </si>
   <si>
     <t xml:space="preserve">Welland</t>
@@ -427,7 +427,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>